<commit_message>
feat(api): implement duplicate detection for file and entry levels
- Add new DuplicateDetectionService to handle file and entry level duplicate checks
- Enhance upload endpoints (OFX and XLSX) with file hash calculation and duplicate verification
- Update UploadHistory model with new fields for tracking duplicates and file hashes
- Modify XLSX processor to detect and skip duplicate entries within files and against existing records
- Include detailed duplicate information in API responses
- Add database migration script for new upload history columns
</commit_message>
<xml_diff>
--- a/samples/Novembro21.xlsx
+++ b/samples/Novembro21.xlsx
@@ -5,19 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\conciliadora\mariaconciliadora-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB43864C-1587-4119-9FAC-0B93EE75DA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C829190-C405-43A6-993F-63CF028B9C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{65131A9D-D158-434C-B873-9478910C6E69}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{65131A9D-D158-434C-B873-9478910C6E69}"/>
   </bookViews>
   <sheets>
     <sheet name="Novembro" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
   <si>
     <t>Saldo</t>
   </si>
@@ -97,25 +93,22 @@
     <t>Mov Tit Cob</t>
   </si>
   <si>
-    <t>Valor para relat mensal</t>
-  </si>
-  <si>
-    <t>Observações:</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Saldo Inicial</t>
+    <t>description</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>observations</t>
+  </si>
+  <si>
+    <t>monthly_report_value</t>
+  </si>
+  <si>
+    <t>tipo</t>
   </si>
 </sst>
 </file>
@@ -149,8 +142,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -171,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -194,37 +187,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -241,74 +217,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Janeiro"/>
-      <sheetName val="Resultado Janeiro"/>
-      <sheetName val="Fevereiro"/>
-      <sheetName val="Resultado Fevereiro"/>
-      <sheetName val="Março"/>
-      <sheetName val="Resultado Março"/>
-      <sheetName val="Abril"/>
-      <sheetName val="Resultado Abril"/>
-      <sheetName val="Maio"/>
-      <sheetName val="Resultado Maio"/>
-      <sheetName val="Junho"/>
-      <sheetName val="Resultado Junho"/>
-      <sheetName val="Julho"/>
-      <sheetName val="Resultado Julho"/>
-      <sheetName val="Agosto"/>
-      <sheetName val="Resultado Agosto"/>
-      <sheetName val="Setembro"/>
-      <sheetName val="Resultado Setembro"/>
-      <sheetName val="Outubro"/>
-      <sheetName val="Resultado Outubro"/>
-      <sheetName val="Resultado Novembro"/>
-      <sheetName val="Dezembro"/>
-      <sheetName val="Resultado Dezembro"/>
-      <sheetName val="Consolidado 2021"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18">
-        <row r="55">
-          <cell r="F55">
-            <v>2519.170000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -574,56 +482,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A484EFEC-336E-4C6E-91D2-D8DB6B0CD2FF}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D31"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="8">
-        <f>[1]Outubro!F55</f>
-        <v>2519.170000000001</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="E1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>44866</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-200</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F30" si="0">IF(D2="Saldo",C2,IF(C2&lt;0,C2*-1,C2))</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>44866</v>
       </c>
@@ -631,76 +545,76 @@
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>-200</v>
+        <v>-1700</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1">
-        <f>IF(D3="Saldo",C3,IF(C3&lt;0,C3*-1,C3))</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>44866</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2">
-        <v>-1700</v>
+        <v>424.93</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
-        <f>IF(D4="Saldo",C4,IF(C4&lt;0,C4*-1,C4))</f>
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>424.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>44866</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2">
-        <v>424.93</v>
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="e">
+        <f>#REF!+C2+C3+C4</f>
+        <v>#REF!</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1">
-        <f>IF(D5="Saldo",C5,IF(C5&lt;0,C5*-1,C5))</f>
-        <v>424.93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
-        <v>44866</v>
+        <v>44868</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" s="2">
-        <f>B1+C3+C4+C5</f>
-        <v>1044.100000000001</v>
+        <v>-500</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <f>IF(D6="Saldo",C6,IF(C6&lt;0,C6*-1,C6))</f>
-        <v>1044.100000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>44868</v>
       </c>
@@ -708,18 +622,18 @@
         <v>2</v>
       </c>
       <c r="C7" s="2">
-        <v>-500</v>
+        <v>-250</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <f>IF(D7="Saldo",C7,IF(C7&lt;0,C7*-1,C7))</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>44868</v>
       </c>
@@ -727,154 +641,154 @@
         <v>2</v>
       </c>
       <c r="C8" s="2">
-        <v>-250</v>
+        <v>-50</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <f>IF(D8="Saldo",C8,IF(C8&lt;0,C8*-1,C8))</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>44868</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2">
-        <v>-50</v>
+        <v>-105</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
-        <f>IF(D9="Saldo",C9,IF(C9&lt;0,C9*-1,C9))</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>44868</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2">
-        <v>-105</v>
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="e">
+        <f>SUM(C5:C9)</f>
+        <v>#REF!</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1">
-        <f>IF(D10="Saldo",C10,IF(C10&lt;0,C10*-1,C10))</f>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
-        <v>44868</v>
+        <v>44869</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2">
-        <f>SUM(C6:C10)</f>
-        <v>139.10000000000105</v>
+        <v>690</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
-        <f>IF(D11="Saldo",C11,IF(C11&lt;0,C11*-1,C11))</f>
-        <v>139.10000000000105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>44869</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="2">
-        <v>690</v>
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="e">
+        <f>SUM(C10:C11)</f>
+        <v>#REF!</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1">
-        <f>IF(D12="Saldo",C12,IF(C12&lt;0,C12*-1,C12))</f>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
-        <v>44869</v>
+        <v>44870</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C13" s="2">
-        <f>SUM(C11:C12)</f>
-        <v>829.10000000000105</v>
+        <v>-310.56</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
-        <f>IF(D13="Saldo",C13,IF(C13&lt;0,C13*-1,C13))</f>
-        <v>829.10000000000105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>310.56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>44870</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="2">
-        <v>-310.56</v>
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="e">
+        <f>SUM(C12:C13)</f>
+        <v>#REF!</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="F14" s="1">
-        <f>IF(D14="Saldo",C14,IF(C14&lt;0,C14*-1,C14))</f>
-        <v>310.56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
-        <v>44870</v>
+        <v>44873</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2">
-        <f>SUM(C13:C14)</f>
-        <v>518.5400000000011</v>
+        <v>-250</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
-        <f>IF(D15="Saldo",C15,IF(C15&lt;0,C15*-1,C15))</f>
-        <v>518.5400000000011</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>44873</v>
       </c>
@@ -882,18 +796,18 @@
         <v>2</v>
       </c>
       <c r="C16" s="2">
-        <v>-250</v>
+        <v>-150</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
-        <f>IF(D16="Saldo",C16,IF(C16&lt;0,C16*-1,C16))</f>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>44873</v>
       </c>
@@ -901,18 +815,18 @@
         <v>2</v>
       </c>
       <c r="C17" s="2">
-        <v>-150</v>
+        <v>-100</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1">
-        <f>IF(D17="Saldo",C17,IF(C17&lt;0,C17*-1,C17))</f>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>44873</v>
       </c>
@@ -920,266 +834,248 @@
         <v>2</v>
       </c>
       <c r="C18" s="2">
-        <v>-100</v>
+        <v>-15</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1">
-        <f>IF(D18="Saldo",C18,IF(C18&lt;0,C18*-1,C18))</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>44873</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2">
-        <v>-15</v>
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="e">
+        <f>SUM(C14:C18)</f>
+        <v>#REF!</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="1">
-        <f>IF(D19="Saldo",C19,IF(C19&lt;0,C19*-1,C19))</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
-        <v>44873</v>
+        <v>44890</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C20" s="2">
-        <f>SUM(C15:C19)</f>
-        <v>3.5400000000011005</v>
+        <v>-1700</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1">
-        <f>IF(D20="Saldo",C20,IF(C20&lt;0,C20*-1,C20))</f>
-        <v>3.5400000000011005</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>44890</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C21" s="2">
-        <v>-1700</v>
+        <v>-2510.9699999999998</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1">
-        <f>IF(D21="Saldo",C21,IF(C21&lt;0,C21*-1,C21))</f>
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>2510.9699999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>44890</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22" s="2">
-        <v>-2510.9699999999998</v>
+        <v>-50.22</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1">
-        <f>IF(D22="Saldo",C22,IF(C22&lt;0,C22*-1,C22))</f>
-        <v>2510.9699999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>50.22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>44890</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="2">
-        <v>-50.22</v>
+        <v>-17.739999999999998</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1">
-        <f>IF(D23="Saldo",C23,IF(C23&lt;0,C23*-1,C23))</f>
-        <v>50.22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>17.739999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>44890</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C24" s="2">
-        <v>-17.739999999999998</v>
+        <v>5064.78</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1">
-        <f>IF(D24="Saldo",C24,IF(C24&lt;0,C24*-1,C24))</f>
-        <v>17.739999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>5064.78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>44890</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="2">
-        <v>5064.78</v>
+        <v>0</v>
+      </c>
+      <c r="C25" s="2" t="e">
+        <f>SUM(C19:C24)</f>
+        <v>#REF!</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1">
-        <f>IF(D25="Saldo",C25,IF(C25&lt;0,C25*-1,C25))</f>
-        <v>5064.78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F25" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
-        <v>44890</v>
+        <v>44894</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C26" s="2">
-        <f>SUM(C20:C25)</f>
-        <v>789.39000000000124</v>
+        <v>-300</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1">
-        <f>IF(D26="Saldo",C26,IF(C26&lt;0,C26*-1,C26))</f>
-        <v>789.39000000000124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>44894</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C27" s="2">
-        <v>-300</v>
+        <v>-177.48</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1">
-        <f>IF(D27="Saldo",C27,IF(C27&lt;0,C27*-1,C27))</f>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>177.48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>44894</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="2">
-        <v>-177.48</v>
+        <v>0</v>
+      </c>
+      <c r="C28" s="2" t="e">
+        <f>SUM(C25:C27)</f>
+        <v>#REF!</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="1">
-        <f>IF(D28="Saldo",C28,IF(C28&lt;0,C28*-1,C28))</f>
-        <v>177.48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F28" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
-        <v>44894</v>
+        <v>44895</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C29" s="2">
-        <f>SUM(C26:C28)</f>
-        <v>311.91000000000122</v>
+        <v>-100</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1">
-        <f>IF(D29="Saldo",C29,IF(C29&lt;0,C29*-1,C29))</f>
-        <v>311.91000000000122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>44895</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="2">
-        <v>-100</v>
+        <v>0</v>
+      </c>
+      <c r="C30" s="2" t="e">
+        <f>SUM(C28:C29)</f>
+        <v>#REF!</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1"/>
-      <c r="F30" s="1">
-        <f>IF(D30="Saldo",C30,IF(C30&lt;0,C30*-1,C30))</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="3">
-        <v>44895</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="2">
-        <f>SUM(C29:C30)</f>
-        <v>211.91000000000122</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1">
-        <f>IF(D31="Saldo",C31,IF(C31&lt;0,C31*-1,C31))</f>
-        <v>211.91000000000122</v>
+      <c r="F30" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update script source in index.html to new version for improved functionality
</commit_message>
<xml_diff>
--- a/samples/Novembro21.xlsx
+++ b/samples/Novembro21.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\conciliadora\mariaconciliadora-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C829190-C405-43A6-993F-63CF028B9C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CBB6C5-E6C0-4CE7-96C5-1713A07F137C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{65131A9D-D158-434C-B873-9478910C6E69}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="25">
-  <si>
-    <t>Saldo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
   <si>
     <t>Retirada Sócio</t>
   </si>
@@ -482,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A484EFEC-336E-4C6E-91D2-D8DB6B0CD2FF}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,60 +492,60 @@
     <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>44866</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>-200</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F30" si="0">IF(D2="Saldo",C2,IF(C2&lt;0,C2*-1,C2))</f>
+        <f t="shared" ref="F2:F22" si="0">IF(D2="Saldo",C2,IF(C2&lt;0,C2*-1,C2))</f>
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>44866</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2">
         <v>-1700</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1">
@@ -556,18 +553,18 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>44866</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2">
         <v>424.93</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
@@ -575,507 +572,347 @@
         <v>424.93</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
-        <v>44866</v>
+        <v>44868</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2" t="e">
-        <f>#REF!+C2+C3+C4</f>
-        <v>#REF!</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>-500</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>44868</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>-500</v>
+        <v>-250</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>44868</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>-250</v>
+        <v>-50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>44868</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2">
-        <v>-50</v>
+        <v>-105</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
-        <v>44868</v>
+        <v>44869</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2">
-        <v>-105</v>
+        <v>690</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
-        <v>44868</v>
+        <v>44870</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2">
+        <v>-310.56</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>310.56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>44873</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-250</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C10" s="2" t="e">
-        <f>SUM(C5:C9)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>44869</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2">
-        <v>690</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
-        <v>44869</v>
+        <v>44873</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2" t="e">
-        <f>SUM(C10:C11)</f>
-        <v>#REF!</v>
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-150</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F12" s="1">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
-        <v>44870</v>
+        <v>44873</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2">
-        <v>-310.56</v>
+        <v>-100</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>310.56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
-        <v>44870</v>
+        <v>44873</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-15</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
+        <v>44890</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-1700</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C14" s="2" t="e">
-        <f>SUM(C12:C13)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>44873</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2">
-        <v>-250</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
-        <v>44873</v>
+        <v>44890</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C16" s="2">
-        <v>-150</v>
+        <v>-2510.9699999999998</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+        <v>2510.9699999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
-        <v>44873</v>
+        <v>44890</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2">
-        <v>-100</v>
+        <v>-50.22</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <v>50.22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
-        <v>44873</v>
+        <v>44890</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2">
-        <v>-15</v>
+        <v>-17.739999999999998</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="K18" s="5"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+        <v>17.739999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
-        <v>44873</v>
+        <v>44890</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>5064.78</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>5064.78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>44894</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-300</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C19" s="2" t="e">
-        <f>SUM(C14:C18)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
-        <v>44890</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="2">
-        <v>-1700</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
-        <v>44890</v>
+        <v>44894</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2">
-        <v>-2510.9699999999998</v>
+        <v>-177.48</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>2510.9699999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+        <v>177.48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
-        <v>44890</v>
+        <v>44895</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2">
-        <v>-50.22</v>
+        <v>-100</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>50.22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
-        <v>44890</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="2">
-        <v>-17.739999999999998</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>17.739999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
-        <v>44890</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="2">
-        <v>5064.78</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1">
-        <f t="shared" si="0"/>
-        <v>5064.78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>44890</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="2" t="e">
-        <f>SUM(C19:C24)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
-        <v>44894</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="2">
-        <v>-300</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
-        <v>44894</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2">
-        <v>-177.48</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1">
-        <f t="shared" si="0"/>
-        <v>177.48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
-        <v>44894</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2" t="e">
-        <f>SUM(C25:C27)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
-        <v>44895</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="2">
-        <v>-100</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1">
-        <f t="shared" si="0"/>
         <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="3">
-        <v>44895</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2" t="e">
-        <f>SUM(C28:C29)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>